<commit_message>
hardware design parts and readme
</commit_message>
<xml_diff>
--- a/Hardware_design_control/Parts_List.xlsx
+++ b/Hardware_design_control/Parts_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\Thesis &amp; Internship\pybeamprofiler\Hardware_design_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E8574DA-7883-4C55-9AC9-7AA9AC6DC860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8388447-B560-4C79-ABD1-6E059F9AE8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24000" yWindow="3570" windowWidth="33050" windowHeight="14200" xr2:uid="{BABFED77-8807-431F-8901-F059BC18269A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Parts</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>https://www.thorlabs.com/thorproduct.cfm?partnumber=KM1CE</t>
+  </si>
+  <si>
+    <t>https://www.loretech.io/products/teledyne-flir-ffy-u3-04s2m-s?variant=41921567195312&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;gclid=CjwKCAjwvfmoBhAwEiwAG2tqzJ1Q4EKml1YO4GNgePSl51jbAo5Rcsx44ZdUebNdtIqEfOWRUJiS6hoCbBUQAvD_BwE</t>
+  </si>
+  <si>
+    <t>Teledyne FLIR FFY-U3-04S2M-S</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07432A9-D084-4406-B1EC-692158496282}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,6 +519,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>